<commit_message>
add rescore function, adjust rois,update screenshots, one fixplot
</commit_message>
<xml_diff>
--- a/ROI/ROI_Final.xlsx
+++ b/ROI/ROI_Final.xlsx
@@ -984,9 +984,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DI96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="AO6" sqref="AO6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,7 +1021,7 @@
     <col min="34" max="35" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="42" max="43" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -2148,7 +2148,7 @@
         <v>273</v>
       </c>
       <c r="AM6" s="8">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="AN6" s="8">
         <v>94</v>

</xml_diff>